<commit_message>
Some changes in samples
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample90-headerinfo-built-in-functions.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample90-headerinfo-built-in-functions.xlsx
@@ -279,22 +279,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="10">
-        <v>42728.7003347569</v>
+        <v>42731.0647456713</v>
       </c>
       <c r="C3" s="10">
-        <v>42728.7003347569</v>
+        <v>42731.0647456713</v>
       </c>
       <c r="D3" s="10">
-        <v>42728.7003347569</v>
+        <v>42731.0647456713</v>
       </c>
       <c r="E3" s="10">
-        <v>42728.7003347569</v>
+        <v>42731.0647456713</v>
       </c>
       <c r="F3" s="10">
-        <v>42728.7003347569</v>
+        <v>42731.0647456713</v>
       </c>
       <c r="G3" s="10">
-        <v>42728.7003347569</v>
+        <v>42731.0647456713</v>
       </c>
     </row>
     <row r="5">

</xml_diff>